<commit_message>
revison de cambios a los modelos de dartos con jcarrillo
</commit_message>
<xml_diff>
--- a/docs/PLAN DE CUENTAS.xlsx
+++ b/docs/PLAN DE CUENTAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardo/Repositorios/ledger/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E683237-39BD-1F40-BD6A-8895E9AB921B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185207F8-79C8-FD4B-81B8-E75BFA100085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="454">
   <si>
     <t>Nº</t>
   </si>
@@ -1371,6 +1371,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>banco internacional</t>
+  </si>
+  <si>
+    <t>Banco Pichcincha</t>
+  </si>
+  <si>
+    <t>xxxx 01</t>
+  </si>
+  <si>
+    <t>xxxx 02</t>
   </si>
 </sst>
 </file>
@@ -4606,7 +4618,7 @@
   <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4756,13 +4768,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>172</v>
+        <v>450</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>443</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4770,13 +4785,16 @@
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>172</v>
+        <v>451</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>443</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4792,6 +4810,9 @@
       <c r="D11" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
@@ -4806,6 +4827,9 @@
       <c r="D12" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -4820,6 +4844,9 @@
       <c r="D13" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
@@ -4834,6 +4861,9 @@
       <c r="D14" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
@@ -4848,6 +4878,9 @@
       <c r="D15" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="9">
@@ -4862,8 +4895,11 @@
       <c r="D16" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -4876,8 +4912,11 @@
       <c r="D17" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -4890,13 +4929,16 @@
       <c r="D18" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="9">
         <v>1102003002</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>170</v>
+        <v>452</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4904,13 +4946,16 @@
       <c r="D19" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="9">
         <v>1102003003</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>170</v>
+        <v>453</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4918,8 +4963,11 @@
       <c r="D20" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="9">
         <v>1102003004</v>
       </c>
@@ -4932,8 +4980,11 @@
       <c r="D21" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -4946,8 +4997,11 @@
       <c r="D22" s="3" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -4961,7 +5015,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="9">
         <v>1103</v>
       </c>
@@ -4975,7 +5029,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="9">
         <v>1103001</v>
       </c>
@@ -4989,7 +5043,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="9">
         <v>1103001001</v>
       </c>
@@ -5003,7 +5057,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="9">
         <v>1104</v>
       </c>
@@ -5017,7 +5071,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="9">
         <v>1104001</v>
       </c>
@@ -5031,7 +5085,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:5" ht="15">
       <c r="A29" s="9">
         <v>1104001001</v>
       </c>
@@ -5045,7 +5099,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -5059,7 +5113,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -5073,7 +5127,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>